<commit_message>
ENGLISH REPORT ALMOST DONE
</commit_message>
<xml_diff>
--- a/ENGLISH/READING FILE/RAPPORT/Vocabulary.xlsx
+++ b/ENGLISH/READING FILE/RAPPORT/Vocabulary.xlsx
@@ -886,7 +886,18 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
         <color auto="1"/>
       </right>
       <top/>
@@ -895,24 +906,13 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
+      <right style="thick">
         <color auto="1"/>
       </right>
       <top/>
       <bottom style="thick">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thick">
-        <color auto="1"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -936,23 +936,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1307,17 +1307,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G191"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G6"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="14.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="13.85546875" customWidth="1"/>
   </cols>
@@ -1361,7 +1361,7 @@
       <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="7" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1384,7 +1384,7 @@
       <c r="F3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G3" s="10"/>
+      <c r="G3" s="8"/>
     </row>
     <row r="4" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -1405,7 +1405,7 @@
       <c r="F4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="10"/>
+      <c r="G4" s="8"/>
     </row>
     <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -1426,7 +1426,7 @@
       <c r="F5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="10"/>
+      <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
@@ -1468,7 +1468,7 @@
       <c r="F7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="7" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1491,7 +1491,7 @@
       <c r="F8" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="G8" s="7"/>
+      <c r="G8" s="10"/>
     </row>
     <row r="9" spans="1:7" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
@@ -1512,7 +1512,7 @@
       <c r="F9" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G9" s="8"/>
+      <c r="G9" s="11"/>
     </row>
     <row r="10" spans="1:7" ht="121.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -1533,7 +1533,7 @@
       <c r="F10" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="7" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1544,7 +1544,7 @@
       <c r="B11" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="6" t="s">
         <v>134</v>
       </c>
       <c r="D11" s="3" t="s">
@@ -1577,7 +1577,7 @@
       <c r="F12" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="7" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1588,7 +1588,7 @@
       <c r="B13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="6" t="s">
         <v>140</v>
       </c>
       <c r="D13" s="3" t="s">
@@ -1600,7 +1600,7 @@
       <c r="F13" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="G13" s="8"/>
+      <c r="G13" s="11"/>
     </row>
     <row r="14" spans="1:7" ht="60.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -1621,7 +1621,7 @@
       <c r="F14" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G14" s="7" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1665,7 +1665,7 @@
       <c r="F16" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="7" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1688,7 +1688,7 @@
       <c r="F17" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G17" s="10"/>
+      <c r="G17" s="8"/>
     </row>
     <row r="18" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -1709,7 +1709,7 @@
       <c r="F18" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G18" s="10"/>
+      <c r="G18" s="8"/>
     </row>
     <row r="19" spans="1:7" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
@@ -1730,7 +1730,7 @@
       <c r="F19" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="G19" s="10"/>
+      <c r="G19" s="8"/>
     </row>
     <row r="20" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
@@ -1751,7 +1751,7 @@
       <c r="F20" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G20" s="10"/>
+      <c r="G20" s="8"/>
     </row>
     <row r="21" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
@@ -1772,7 +1772,7 @@
       <c r="F21" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G21" s="10"/>
+      <c r="G21" s="8"/>
     </row>
     <row r="22" spans="1:7" ht="150" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
@@ -1793,7 +1793,7 @@
       <c r="F22" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="G22" s="10"/>
+      <c r="G22" s="8"/>
     </row>
     <row r="23" spans="1:7" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -1814,7 +1814,7 @@
       <c r="F23" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="G23" s="10"/>
+      <c r="G23" s="8"/>
     </row>
     <row r="24" spans="1:7" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
@@ -1835,7 +1835,7 @@
       <c r="F24" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="G24" s="10"/>
+      <c r="G24" s="8"/>
     </row>
     <row r="25" spans="1:7" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
@@ -1856,7 +1856,7 @@
       <c r="F25" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G25" s="10"/>
+      <c r="G25" s="8"/>
     </row>
     <row r="26" spans="1:7" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
@@ -1877,7 +1877,7 @@
       <c r="F26" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="G26" s="10"/>
+      <c r="G26" s="8"/>
     </row>
     <row r="27" spans="1:7" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
@@ -1898,7 +1898,7 @@
       <c r="F27" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="G27" s="10"/>
+      <c r="G27" s="8"/>
     </row>
     <row r="28" spans="1:7" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
@@ -1919,7 +1919,7 @@
       <c r="F28" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="G28" s="10"/>
+      <c r="G28" s="8"/>
     </row>
     <row r="29" spans="1:7" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
@@ -1940,7 +1940,7 @@
       <c r="F29" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="G29" s="10"/>
+      <c r="G29" s="8"/>
     </row>
     <row r="30" spans="1:7" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
@@ -1961,7 +1961,7 @@
       <c r="F30" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="G30" s="10"/>
+      <c r="G30" s="8"/>
     </row>
     <row r="31" spans="1:7" ht="98.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
@@ -2003,7 +2003,7 @@
       <c r="F32" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="G32" s="6" t="s">
+      <c r="G32" s="7" t="s">
         <v>121</v>
       </c>
     </row>
@@ -2026,7 +2026,7 @@
       <c r="F33" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G33" s="7"/>
+      <c r="G33" s="10"/>
     </row>
     <row r="34" spans="1:7" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
@@ -2047,7 +2047,7 @@
       <c r="F34" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="G34" s="7"/>
+      <c r="G34" s="10"/>
     </row>
     <row r="35" spans="1:7" ht="125.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
@@ -2068,7 +2068,7 @@
       <c r="F35" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="G35" s="7"/>
+      <c r="G35" s="10"/>
     </row>
     <row r="36" spans="1:7" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
@@ -2089,7 +2089,7 @@
       <c r="F36" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="G36" s="7"/>
+      <c r="G36" s="10"/>
     </row>
     <row r="37" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
@@ -2110,7 +2110,7 @@
       <c r="F37" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="G37" s="7"/>
+      <c r="G37" s="10"/>
     </row>
     <row r="38" spans="1:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
@@ -2131,7 +2131,7 @@
       <c r="F38" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="G38" s="7"/>
+      <c r="G38" s="10"/>
     </row>
     <row r="39" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
@@ -2152,7 +2152,7 @@
       <c r="F39" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="G39" s="7"/>
+      <c r="G39" s="10"/>
     </row>
     <row r="40" spans="1:7" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
@@ -2173,7 +2173,7 @@
       <c r="F40" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="G40" s="7"/>
+      <c r="G40" s="10"/>
     </row>
     <row r="41" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
@@ -2194,7 +2194,7 @@
       <c r="F41" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="G41" s="7"/>
+      <c r="G41" s="10"/>
     </row>
     <row r="42" spans="1:7" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
@@ -2215,7 +2215,7 @@
       <c r="F42" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="G42" s="7"/>
+      <c r="G42" s="10"/>
     </row>
     <row r="43" spans="1:7" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
@@ -2236,7 +2236,7 @@
       <c r="F43" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="G43" s="7"/>
+      <c r="G43" s="10"/>
     </row>
     <row r="44" spans="1:7" ht="153.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
@@ -2257,7 +2257,7 @@
       <c r="F44" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="G44" s="7"/>
+      <c r="G44" s="10"/>
     </row>
     <row r="45" spans="1:7" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
@@ -2278,7 +2278,7 @@
       <c r="F45" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="G45" s="7"/>
+      <c r="G45" s="10"/>
     </row>
     <row r="46" spans="1:7" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
@@ -2299,7 +2299,7 @@
       <c r="F46" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="G46" s="7"/>
+      <c r="G46" s="10"/>
     </row>
     <row r="47" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
@@ -2320,7 +2320,7 @@
       <c r="F47" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="G47" s="7"/>
+      <c r="G47" s="10"/>
     </row>
     <row r="48" spans="1:7" ht="81" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
@@ -2341,7 +2341,7 @@
       <c r="F48" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="G48" s="7"/>
+      <c r="G48" s="10"/>
     </row>
     <row r="49" spans="1:7" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
@@ -2362,7 +2362,7 @@
       <c r="F49" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="G49" s="7"/>
+      <c r="G49" s="10"/>
     </row>
     <row r="50" spans="1:7" ht="187.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
@@ -2383,7 +2383,7 @@
       <c r="F50" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="G50" s="7"/>
+      <c r="G50" s="10"/>
     </row>
     <row r="51" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
@@ -2404,7 +2404,7 @@
       <c r="F51" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="G51" s="7"/>
+      <c r="G51" s="10"/>
     </row>
     <row r="52" spans="1:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
@@ -2425,7 +2425,7 @@
       <c r="F52" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="G52" s="8"/>
+      <c r="G52" s="11"/>
     </row>
     <row r="53" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="G53" s="4"/>

</xml_diff>